<commit_message>
screenshots of k-maps added
</commit_message>
<xml_diff>
--- a/labs/02-logic/k maps.xlsx
+++ b/labs/02-logic/k maps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakub\Desktop\škola\de1\cp\digital-electronics-1\digital-electronics-1\labs\02-logic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD43356C-E18F-4C39-AC78-CA06ADD7C036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BA3CEF-4146-492E-B5AA-B4ADA8762979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2500" windowWidth="14400" windowHeight="7360" xr2:uid="{95A68B64-63DA-42EC-A318-B7DBD87722ED}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{95A68B64-63DA-42EC-A318-B7DBD87722ED}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>00</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t>B&gt;A</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
   <si>
     <t>B&lt;A</t>
@@ -103,15 +97,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -120,13 +160,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,222 +489,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815B0709-396B-42D3-93D1-123AAD8994F5}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="C4:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="9" width="4.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E1" t="s">
+    <row r="4" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="E6" s="1"/>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="E7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C10" s="9"/>
+      <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C6" s="1" t="s">
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="E18" s="7"/>
+      <c r="F18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C7" s="1" t="s">
+      <c r="I18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="E19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="D20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C21" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C22" s="9"/>
+      <c r="E22" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="C16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="F11:G11"/>
+  <mergeCells count="8">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C9:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E7:E10 F6:I6 F18:I18 E19:E22" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>